<commit_message>
Update to showcase all variations currently possible
</commit_message>
<xml_diff>
--- a/BatchInput.xlsx
+++ b/BatchInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\WeightedLatticeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4B21BC-59A8-4245-A2BD-7E715E665F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B072A2-E559-4326-B4E5-8D99476F7C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6582" yWindow="6204" windowWidth="23232" windowHeight="12552" xr2:uid="{2196279D-7537-40B7-BC00-A2BA768C1593}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{2196279D-7537-40B7-BC00-A2BA768C1593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,7 +104,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC26A4B1-DC33-4AAE-AC36-6AE0086903DD}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H6"/>
+      <selection activeCell="F10" sqref="F10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +430,7 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -462,76 +462,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3.996003996003996E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3.996003996003996E-2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3.996003996003996E-2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3.996003996003996E-2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3.996003996003996E-2</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
       <c r="D3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1">
-        <v>4.5954045954045952E-2</v>
+        <v>3.996003996003996E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>4.5954045954045952E-2</v>
+        <v>3.996003996003996E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>4.5954045954045952E-2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -543,22 +543,22 @@
         <v>2</v>
       </c>
       <c r="F4" s="1">
-        <v>7.992007992007992E-2</v>
+        <v>3.996003996003996E-2</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>3.996003996003996E-2</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -616,9 +616,170 @@
         <v>0</v>
       </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>0.5</v>
       </c>
-      <c r="J6">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3.996003996003996E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.996003996003996E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3.996003996003996E-2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4.5954045954045952E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.5954045954045952E-2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.5954045954045952E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4.5954045954045952E-2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.5954045954045952E-2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4.5954045954045952E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4.5954045954045952E-2</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7.992007992007992E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to include all examples
</commit_message>
<xml_diff>
--- a/BatchInput.xlsx
+++ b/BatchInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\WeightedLatticeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B072A2-E559-4326-B4E5-8D99476F7C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F87EB2-559B-4142-A981-EB2DFFC9C9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{2196279D-7537-40B7-BC00-A2BA768C1593}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:H10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="K6" s="1"/>
     </row>

</xml_diff>